<commit_message>
+Started with uber login
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7112AAA-2057-4D97-A25D-C23E9B44C668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5447CC5C-7B12-4D56-930E-DE5560CE8344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -180,10 +180,19 @@
     <t>OlaUserName</t>
   </si>
   <si>
-    <t>OlaOTP</t>
-  </si>
-  <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>https://book.olacabs.com/profile?</t>
+  </si>
+  <si>
+    <t>OlaProfile</t>
+  </si>
+  <si>
+    <t>https://m.uber.com/</t>
+  </si>
+  <si>
+    <t>UberUrl</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -619,7 +628,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1648,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1845,18 +1854,25 @@
         <v>46</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20">
-        <v>1047</v>
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2823,7 +2839,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+worked on uber login page
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5447CC5C-7B12-4D56-930E-DE5560CE8344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADE43E5-409F-4A29-9A1A-42DE139EA1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>UberUrl</t>
+  </si>
+  <si>
+    <t>https://riders.uber.com/profile</t>
+  </si>
+  <si>
+    <t>UberProfile</t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1879,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
+Worked on Uber operations
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851D8BF0-900A-47EF-AECF-A6EDB4C72A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A45D2E-E51F-4569-BF1C-CF1FFFD3F17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>UberProfile</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps</t>
+  </si>
+  <si>
+    <t>GoogleMaps</t>
+  </si>
+  <si>
+    <t>UberData</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>DelayUberInput</t>
   </si>
 </sst>
 </file>
@@ -256,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +282,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +652,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -644,7 +662,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1665,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1887,9 +1907,30 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
+worked on ola operations
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A45D2E-E51F-4569-BF1C-CF1FFFD3F17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E56C0D-EFBB-40DB-9FD8-D1A2B60F1BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -214,6 +214,24 @@
   </si>
   <si>
     <t>DelayUberInput</t>
+  </si>
+  <si>
+    <t>Data\Output\Route Tracker-Output.xlsx</t>
+  </si>
+  <si>
+    <t>OutputFile</t>
+  </si>
+  <si>
+    <t>UberCarCost</t>
+  </si>
+  <si>
+    <t>OutputSheet2</t>
+  </si>
+  <si>
+    <t>OlaCarCost</t>
+  </si>
+  <si>
+    <t>OutputSheet1</t>
   </si>
 </sst>
 </file>
@@ -1683,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1931,9 +1949,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2892,7 +2931,6 @@
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+Worked on merging the results
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E56C0D-EFBB-40DB-9FD8-D1A2B60F1BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E4B23-8F6B-488F-ADCA-B250212188FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>OutputSheet1</t>
+  </si>
+  <si>
+    <t>MergedPrices</t>
+  </si>
+  <si>
+    <t>JoinedPrices</t>
+  </si>
+  <si>
+    <t>MergedResultSheet</t>
+  </si>
+  <si>
+    <t>JoinedResultSheet</t>
   </si>
 </sst>
 </file>
@@ -1703,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1973,8 +1985,22 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
+Worked on annotations and exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Capstone_4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E4B23-8F6B-488F-ADCA-B250212188FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B738261-3F31-4C39-AA5C-B315F864CF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -207,9 +207,6 @@
     <t>GoogleMaps</t>
   </si>
   <si>
-    <t>UberData</t>
-  </si>
-  <si>
     <t>Delay</t>
   </si>
   <si>
@@ -234,23 +231,35 @@
     <t>OutputSheet1</t>
   </si>
   <si>
-    <t>MergedPrices</t>
-  </si>
-  <si>
-    <t>JoinedPrices</t>
-  </si>
-  <si>
     <t>MergedResultSheet</t>
   </si>
   <si>
     <t>JoinedResultSheet</t>
+  </si>
+  <si>
+    <t>UberMail</t>
+  </si>
+  <si>
+    <t>UberName</t>
+  </si>
+  <si>
+    <t>UberLastName</t>
+  </si>
+  <si>
+    <t>MergedPrices1</t>
+  </si>
+  <si>
+    <t>JoinedPrices1</t>
+  </si>
+  <si>
+    <t>OlaData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -280,6 +289,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF182027"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -301,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,6 +329,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -330,6 +351,119 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -631,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -682,7 +816,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -1715,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1947,7 +2081,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1955,7 +2089,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -1963,42 +2097,42 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
         <v>66</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2964,7 +3098,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3031,9 +3166,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4032,5 +4188,59 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>